<commit_message>
Adaugare sortare si citire din excel
</commit_message>
<xml_diff>
--- a/out/production/Project3/Room.xlsx
+++ b/out/production/Project3/Room.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24617"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24628"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60D0D9C9-3F8B-40AC-A80D-3F88BEBC9469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EF016AB-9F01-421E-BFE6-8175761D1DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
     <t>#4124</t>
   </si>
   <si>
-    <t>&amp;5325</t>
+    <t>feasgd</t>
   </si>
   <si>
     <t>XL</t>
@@ -523,7 +523,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G16"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Terminat AdminLogin,User Login, alte updaturi.
</commit_message>
<xml_diff>
--- a/out/production/Project3/Room.xlsx
+++ b/out/production/Project3/Room.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
   <si>
     <t>NrCam</t>
   </si>
@@ -149,12 +149,16 @@
   </si>
   <si>
     <t>&amp;5339</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -571,7 +575,7 @@
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7">

</xml_diff>